<commit_message>
fix according to mentors comment
</commit_message>
<xml_diff>
--- a/normalization.xlsx
+++ b/normalization.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="27">
   <si>
     <t>Номер замовлення</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>Таблиця клієнтів</t>
+  </si>
+  <si>
+    <t>Таблиця  товарів</t>
   </si>
 </sst>
 </file>
@@ -178,7 +181,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -473,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:G53"/>
+  <dimension ref="B2:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E53" sqref="E53"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -948,25 +953,39 @@
       </c>
       <c r="E47" s="7"/>
     </row>
-    <row r="49" spans="2:3">
-      <c r="B49" s="8"/>
-      <c r="C49" s="8"/>
-    </row>
-    <row r="50" spans="2:3">
-      <c r="B50" s="6"/>
-      <c r="C50" s="8"/>
-    </row>
-    <row r="51" spans="2:3">
-      <c r="B51" s="6"/>
-      <c r="C51" s="8"/>
-    </row>
-    <row r="52" spans="2:3">
-      <c r="B52" s="6"/>
-      <c r="C52" s="8"/>
-    </row>
-    <row r="53" spans="2:3">
-      <c r="B53" s="6"/>
-      <c r="C53" s="8"/>
+    <row r="49" spans="2:4">
+      <c r="B49" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4">
+      <c r="B50" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D50" s="8"/>
+    </row>
+    <row r="51" spans="2:4">
+      <c r="B51" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D51" s="6"/>
+    </row>
+    <row r="52" spans="2:4">
+      <c r="B52" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D52" s="6"/>
+    </row>
+    <row r="53" spans="2:4">
+      <c r="B53" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D53" s="6"/>
+    </row>
+    <row r="54" spans="2:4">
+      <c r="B54" s="6"/>
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>